<commit_message>
updates to optimal window score table
</commit_message>
<xml_diff>
--- a/visuals_8_sec_vs_optimalwindowscoretable.xlsx
+++ b/visuals_8_sec_vs_optimalwindowscoretable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\ids_svm_slidingwindow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8310FD0-B803-47AE-A923-3A5DDCE85D62}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B462B635-FB48-4C82-AFD2-5206D577C35D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35670" yWindow="1815" windowWidth="12150" windowHeight="11385" xr2:uid="{BEECDDA4-06AE-4594-96BC-5192767F1C9D}"/>
+    <workbookView xWindow="6135" yWindow="1005" windowWidth="18165" windowHeight="15090" xr2:uid="{BEECDDA4-06AE-4594-96BC-5192767F1C9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,19 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
-  <si>
-    <t>DoS</t>
-  </si>
-  <si>
-    <t>Probe</t>
-  </si>
-  <si>
-    <t>U2R</t>
-  </si>
-  <si>
-    <t>R2L</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Change</t>
   </si>
@@ -54,14 +42,45 @@
     <t>F1 for top 6 8 sec windows</t>
   </si>
   <si>
-    <t>Avg F1 improvement</t>
+    <t>DoS Split 1</t>
+  </si>
+  <si>
+    <t>DoS Split 2</t>
+  </si>
+  <si>
+    <t>Probe Split 1</t>
+  </si>
+  <si>
+    <t>Probe Split 2</t>
+  </si>
+  <si>
+    <t>U2R Split 1</t>
+  </si>
+  <si>
+    <t>R2L Split 1</t>
+  </si>
+  <si>
+    <t>U2R Split 2</t>
+  </si>
+  <si>
+    <t>R2L Split 2</t>
+  </si>
+  <si>
+    <t>Percent Change</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,14 +106,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -409,62 +431,71 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="3" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>0.168192771084337</v>
       </c>
       <c r="C2">
-        <v>0.237002341920374</v>
+        <v>0.27579990986931002</v>
       </c>
       <c r="D2">
         <f>C2:C9-B2:B9</f>
-        <v>6.8809570836037004E-2</v>
+        <v>0.10760713878497302</v>
+      </c>
+      <c r="E2" s="1">
+        <f>D2/B2</f>
+        <v>0.63978456440922493</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>0.164343715913222</v>
       </c>
       <c r="C3">
-        <v>0.209980190548061</v>
+        <v>0.21095178519872901</v>
       </c>
       <c r="D3">
         <f>C2:C9-B2:B9</f>
-        <v>4.5636474634838997E-2</v>
+        <v>4.6608069285507009E-2</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E9" si="0">D3/B3</f>
+        <v>0.28360116495185828</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>9.2208182912154005E-2</v>
@@ -476,10 +507,14 @@
         <f>C2:C9-B2:B9</f>
         <v>2.6609609903051001E-2</v>
       </c>
+      <c r="E4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.28858187053096757</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>0.123213915924622</v>
@@ -491,25 +526,33 @@
         <f>C2:C9-B2:B9</f>
         <v>-2.0351167163529943E-3</v>
       </c>
+      <c r="E5" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.6516938862636329E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>0.211767920575644</v>
       </c>
       <c r="C6">
-        <v>0.25455541855048602</v>
+        <v>0.25427135678391899</v>
       </c>
       <c r="D6">
         <f>C2:C9-B2:B9</f>
-        <v>4.278749797484202E-2</v>
+        <v>4.2503436208274986E-2</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.20070762414221591</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>0.17136777783839799</v>
@@ -521,10 +564,14 @@
         <f>C2:C9-B2:B9</f>
         <v>3.2578040771731015E-2</v>
       </c>
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.19010598831743342</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>9.7345597897503203E-2</v>
@@ -536,10 +583,14 @@
         <f>C2:C9-B2:B9</f>
         <v>4.21166575067808E-2</v>
       </c>
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.4326508688264068</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>8.2275084957968106E-2</v>
@@ -551,9 +602,9 @@
         <f>C2:C9-B2:B9</f>
         <v>4.30189814356879E-2</v>
       </c>
-      <c r="E9">
-        <f>AVERAGE(D2:D9)</f>
-        <v>3.7440214543326966E-2</v>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.52286766349332869</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add F1 score table
</commit_message>
<xml_diff>
--- a/visuals_8_sec_vs_optimalwindowscoretable.xlsx
+++ b/visuals_8_sec_vs_optimalwindowscoretable.xlsx
@@ -1,78 +1,72 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\ids_svm_slidingwindow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mountrouidoux/Documents/GitHub/ids_svm_slidingwindow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B462B635-FB48-4C82-AFD2-5206D577C35D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C3739D-DC0A-B34A-A6EE-412F6154247C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6135" yWindow="1005" windowWidth="18165" windowHeight="15090" xr2:uid="{BEECDDA4-06AE-4594-96BC-5192767F1C9D}"/>
+    <workbookView xWindow="6140" yWindow="1000" windowWidth="18160" windowHeight="15100" xr2:uid="{BEECDDA4-06AE-4594-96BC-5192767F1C9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Change</t>
-  </si>
-  <si>
-    <t>Optimal Time Windows</t>
-  </si>
-  <si>
-    <t>F1 for top 6 8 sec windows</t>
-  </si>
-  <si>
-    <t>DoS Split 1</t>
-  </si>
-  <si>
-    <t>DoS Split 2</t>
-  </si>
-  <si>
-    <t>Probe Split 1</t>
-  </si>
-  <si>
-    <t>Probe Split 2</t>
-  </si>
-  <si>
-    <t>U2R Split 1</t>
-  </si>
-  <si>
-    <t>R2L Split 1</t>
-  </si>
-  <si>
-    <t>U2R Split 2</t>
-  </si>
-  <si>
-    <t>R2L Split 2</t>
-  </si>
-  <si>
-    <t>Percent Change</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Top 6 8-sec split 1</t>
+  </si>
+  <si>
+    <t>Top 6 8-sec split 2</t>
+  </si>
+  <si>
+    <t>Optimal TW split1</t>
+  </si>
+  <si>
+    <t>Optimal TW split2</t>
+  </si>
+  <si>
+    <t>% Change split1</t>
+  </si>
+  <si>
+    <t>% Change split2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DoS </t>
+  </si>
+  <si>
+    <t>Probe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2R </t>
+  </si>
+  <si>
+    <t>R2L</t>
+  </si>
+  <si>
+    <t>Attack Type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -110,9 +104,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,182 +423,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34B57C41-1716-4930-8E4B-421FABB7C175}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="3" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="4" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2">
         <v>0.168192771084337</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
+        <v>0.164343715913222</v>
+      </c>
+      <c r="D2" s="2">
         <v>0.27579990986931002</v>
       </c>
-      <c r="D2">
-        <f>C2:C9-B2:B9</f>
-        <v>0.10760713878497302</v>
-      </c>
-      <c r="E2" s="1">
-        <f>D2/B2</f>
+      <c r="E2" s="2">
+        <v>0.21095178519872901</v>
+      </c>
+      <c r="F2" s="1">
+        <f>(D2-B2)/B2</f>
         <v>0.63978456440922493</v>
       </c>
+      <c r="G2" s="1">
+        <f>(E2-C2)/C2</f>
+        <v>0.28360116495185828</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>0.164343715913222</v>
-      </c>
-      <c r="C3">
-        <v>0.21095178519872901</v>
-      </c>
-      <c r="D3">
-        <f>C2:C9-B2:B9</f>
-        <v>4.6608069285507009E-2</v>
-      </c>
-      <c r="E3" s="1">
-        <f t="shared" ref="E3:E9" si="0">D3/B3</f>
-        <v>0.28360116495185828</v>
+        <v>7</v>
+      </c>
+      <c r="B3" s="2">
+        <v>9.2208182912154005E-2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.123213915924622</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.11881779281520501</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.121178799208269</v>
+      </c>
+      <c r="F3" s="1">
+        <f t="shared" ref="F3:F5" si="0">(D3-B3)/B3</f>
+        <v>0.28858187053096757</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" ref="G3:G5" si="1">(E3-C3)/C3</f>
+        <v>-1.6516938862636329E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>9.2208182912154005E-2</v>
-      </c>
-      <c r="C4">
-        <v>0.11881779281520501</v>
-      </c>
-      <c r="D4">
-        <f>C2:C9-B2:B9</f>
-        <v>2.6609609903051001E-2</v>
-      </c>
-      <c r="E4" s="1">
-        <f t="shared" si="0"/>
-        <v>0.28858187053096757</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>0.123213915924622</v>
-      </c>
-      <c r="C5">
-        <v>0.121178799208269</v>
-      </c>
-      <c r="D5">
-        <f>C2:C9-B2:B9</f>
-        <v>-2.0351167163529943E-3</v>
-      </c>
-      <c r="E5" s="1">
-        <f t="shared" si="0"/>
-        <v>-1.6516938862636329E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2">
         <v>0.211767920575644</v>
       </c>
-      <c r="C6">
+      <c r="C4" s="2">
+        <v>0.17136777783839799</v>
+      </c>
+      <c r="D4" s="2">
         <v>0.25427135678391899</v>
       </c>
-      <c r="D6">
-        <f>C2:C9-B2:B9</f>
-        <v>4.2503436208274986E-2</v>
-      </c>
-      <c r="E6" s="1">
+      <c r="E4" s="2">
+        <v>0.203945818610129</v>
+      </c>
+      <c r="F4" s="1">
         <f t="shared" si="0"/>
         <v>0.20070762414221591</v>
       </c>
+      <c r="G4" s="1">
+        <f t="shared" si="1"/>
+        <v>0.19010598831743342</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
-        <v>0.17136777783839799</v>
-      </c>
-      <c r="C7">
-        <v>0.203945818610129</v>
-      </c>
-      <c r="D7">
-        <f>C2:C9-B2:B9</f>
-        <v>3.2578040771731015E-2</v>
-      </c>
-      <c r="E7" s="1">
-        <f t="shared" si="0"/>
-        <v>0.19010598831743342</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
+      <c r="B5" s="2">
         <v>9.7345597897503203E-2</v>
       </c>
-      <c r="C8">
+      <c r="C5" s="2">
+        <v>8.2275084957968106E-2</v>
+      </c>
+      <c r="D5" s="2">
         <v>0.139462255404284</v>
       </c>
-      <c r="D8">
-        <f>C2:C9-B2:B9</f>
-        <v>4.21166575067808E-2</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="E5" s="2">
+        <v>0.12529406639365601</v>
+      </c>
+      <c r="F5" s="1">
         <f t="shared" si="0"/>
         <v>0.4326508688264068</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>8.2275084957968106E-2</v>
-      </c>
-      <c r="C9">
-        <v>0.12529406639365601</v>
-      </c>
-      <c r="D9">
-        <f>C2:C9-B2:B9</f>
-        <v>4.30189814356879E-2</v>
-      </c>
-      <c r="E9" s="1">
-        <f t="shared" si="0"/>
+      <c r="G5" s="1">
+        <f t="shared" si="1"/>
         <v>0.52286766349332869</v>
       </c>
     </row>

</xml_diff>